<commit_message>
Atualização de bases das ligas, do dia: 22-04-2024 às 07:46
</commit_message>
<xml_diff>
--- a/Argentina Liga Prefesional/Argentina Liga Prefesional.xlsx
+++ b/Argentina Liga Prefesional/Argentina Liga Prefesional.xlsx
@@ -14,15 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>id</t>
   </si>
   <si>
     <t>Div</t>
-  </si>
-  <si>
-    <t>Div Original Name</t>
   </si>
   <si>
     <t>Date</t>
@@ -455,13 +452,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:AC1"/>
+  <dimension ref="B1:AB1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:29">
+    <row r="1" spans="2:28">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -542,9 +539,6 @@
       </c>
       <c r="AB1" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 27-05-2024 às 07:46
</commit_message>
<xml_diff>
--- a/Argentina Liga Prefesional/Argentina Liga Prefesional.xlsx
+++ b/Argentina Liga Prefesional/Argentina Liga Prefesional.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>id</t>
   </si>
@@ -35,6 +35,12 @@
   </si>
   <si>
     <t>FTAG</t>
+  </si>
+  <si>
+    <t>ht_goals_h</t>
+  </si>
+  <si>
+    <t>ht_goals_a</t>
   </si>
   <si>
     <t>FTR</t>
@@ -452,13 +458,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:AB1"/>
+  <dimension ref="B1:AD1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:28">
+    <row r="1" spans="2:30">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -539,6 +545,12 @@
       </c>
       <c r="AB1" s="1" t="s">
         <v>26</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 30-05-2024 às 23:16
</commit_message>
<xml_diff>
--- a/Argentina Liga Prefesional/Argentina Liga Prefesional.xlsx
+++ b/Argentina Liga Prefesional/Argentina Liga Prefesional.xlsx
@@ -37,10 +37,10 @@
     <t>FTAG</t>
   </si>
   <si>
-    <t>ht_goals_h</t>
-  </si>
-  <si>
-    <t>ht_goals_a</t>
+    <t>HTHG</t>
+  </si>
+  <si>
+    <t>HTAG</t>
   </si>
   <si>
     <t>FTR</t>

</xml_diff>